<commit_message>
Example file for L inverse calculation is updated
</commit_message>
<xml_diff>
--- a/data/Example_Leontief_inverse_calculation.xlsx
+++ b/data/Example_Leontief_inverse_calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="7" r:id="rId1"/>
@@ -1113,7 +1113,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E6" sqref="E6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,9 +1645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1921,19 +1919,19 @@
         <v>210</v>
       </c>
       <c r="M8" s="17">
-        <v>106323.30801193547</v>
+        <v>107505.47667736365</v>
       </c>
       <c r="N8" s="17">
         <v>16103.213972799878</v>
       </c>
       <c r="O8" s="13">
-        <v>3644.0177900101125</v>
+        <v>1308.0435919927895</v>
       </c>
       <c r="P8" s="13">
         <v>195.93146785278896</v>
       </c>
       <c r="Q8" s="13">
-        <v>0</v>
+        <v>1153.8055325891473</v>
       </c>
       <c r="S8" s="20"/>
       <c r="T8" s="1"/>
@@ -1976,19 +1974,19 @@
         <v>25037</v>
       </c>
       <c r="M9" s="19">
-        <v>2105933.2445719279</v>
+        <v>1474543.7225576744</v>
       </c>
       <c r="N9" s="19">
         <v>632906.35752765276</v>
       </c>
       <c r="O9" s="15">
-        <v>208239.87900312577</v>
+        <v>75687.804288948028</v>
       </c>
       <c r="P9" s="15">
         <v>32486.857994751856</v>
       </c>
       <c r="Q9" s="15">
-        <v>0</v>
+        <v>763941.59672843106</v>
       </c>
       <c r="S9" s="20"/>
       <c r="T9" s="1"/>
@@ -2031,19 +2029,19 @@
         <v>115</v>
       </c>
       <c r="M10" s="19">
-        <v>53676.343922698812</v>
+        <v>51285.594170836637</v>
       </c>
       <c r="N10" s="19">
         <v>1182390.8948782317</v>
       </c>
       <c r="O10" s="15">
-        <v>33.814618238095967</v>
+        <v>12.6499589841122</v>
       </c>
       <c r="P10" s="15">
         <v>291.64517961074347</v>
       </c>
       <c r="Q10" s="15">
-        <v>0</v>
+        <v>2411.9144111161586</v>
       </c>
       <c r="S10" s="20"/>
       <c r="T10" s="1"/>
@@ -2086,19 +2084,19 @@
         <v>118935</v>
       </c>
       <c r="M11" s="19">
-        <v>7048312.6373048685</v>
+        <v>6870975.4274285519</v>
       </c>
       <c r="N11" s="19">
         <v>494454.62593600858</v>
       </c>
       <c r="O11" s="15">
-        <v>106436.84578341726</v>
+        <v>49187.589449195468</v>
       </c>
       <c r="P11" s="15">
         <v>3539.6766294211593</v>
       </c>
       <c r="Q11" s="15">
-        <v>0</v>
+        <v>234586.46621053852</v>
       </c>
       <c r="S11" s="20"/>
       <c r="T11" s="1"/>
@@ -2147,13 +2145,13 @@
         <v>819.49375627442464</v>
       </c>
       <c r="O12" s="19">
-        <v>48683.249698980326</v>
+        <v>40502.66470631156</v>
       </c>
       <c r="P12" s="19">
         <v>-33.564392557460792</v>
       </c>
       <c r="Q12" s="15">
-        <v>0</v>
+        <v>8180.5849926687661</v>
       </c>
       <c r="S12" s="20"/>
       <c r="T12" s="1"/>
@@ -2202,13 +2200,13 @@
         <v>80809.185823161592</v>
       </c>
       <c r="O13" s="19">
-        <v>1149202.8091295597</v>
+        <v>1075890.5722947831</v>
       </c>
       <c r="P13" s="19">
         <v>375081.30807734397</v>
       </c>
       <c r="Q13" s="15">
-        <v>0</v>
+        <v>73312.236834776588</v>
       </c>
       <c r="S13" s="20"/>
       <c r="T13" s="1"/>
@@ -2257,13 +2255,13 @@
         <v>10</v>
       </c>
       <c r="O14" s="19">
-        <v>45.404385260888375</v>
+        <v>0</v>
       </c>
       <c r="P14" s="19">
         <v>879077.25282743527</v>
       </c>
       <c r="Q14" s="15">
-        <v>0</v>
+        <v>45.404385260888375</v>
       </c>
       <c r="S14" s="20"/>
       <c r="T14" s="1"/>
@@ -2312,13 +2310,13 @@
         <v>4220.0397558438808</v>
       </c>
       <c r="O15" s="19">
-        <v>7378638.9453427522</v>
+        <v>7260288.2363079153</v>
       </c>
       <c r="P15" s="19">
         <v>470917.6438234222</v>
       </c>
       <c r="Q15" s="15">
-        <v>0</v>
+        <v>118350.70903483592</v>
       </c>
       <c r="S15" s="20"/>
       <c r="T15" s="1"/>
@@ -2331,40 +2329,40 @@
         <v>43</v>
       </c>
       <c r="E16" s="14">
-        <v>0</v>
+        <v>3392.9713519421675</v>
       </c>
       <c r="F16" s="15">
-        <v>0</v>
+        <v>197334.18558686029</v>
       </c>
       <c r="G16" s="15">
-        <v>0</v>
+        <v>12743.89411571547</v>
       </c>
       <c r="H16" s="15">
-        <v>0</v>
+        <v>158355.58075858228</v>
       </c>
       <c r="I16" s="15">
-        <v>0</v>
+        <v>5907.1633783290745</v>
       </c>
       <c r="J16" s="15">
-        <v>0</v>
+        <v>308796.03558555245</v>
       </c>
       <c r="K16" s="15">
-        <v>0</v>
+        <v>31427.424968989566</v>
       </c>
       <c r="L16" s="15">
-        <v>0</v>
+        <v>151474.85676760226</v>
       </c>
       <c r="M16" s="15">
-        <v>0</v>
+        <v>153449.63972739296</v>
       </c>
       <c r="N16" s="15">
-        <v>0</v>
+        <v>86963.012198008553</v>
       </c>
       <c r="O16" s="15">
-        <v>0</v>
+        <v>3520149.4394018687</v>
       </c>
       <c r="P16" s="15">
-        <v>0</v>
+        <v>989188.49839271954</v>
       </c>
       <c r="Q16" s="1"/>
     </row>
@@ -2376,16 +2374,16 @@
         <v>41</v>
       </c>
       <c r="E17" s="14">
-        <v>0</v>
+        <v>6710.2411205275657</v>
       </c>
       <c r="F17" s="15">
-        <v>0</v>
+        <v>74985.055966575514</v>
       </c>
       <c r="G17" s="15">
-        <v>0</v>
+        <v>17099.420776746472</v>
       </c>
       <c r="H17" s="15">
-        <v>0</v>
+        <v>271017.71884496155</v>
       </c>
       <c r="I17" s="15">
         <v>0</v>
@@ -2400,10 +2398,10 @@
         <v>0</v>
       </c>
       <c r="M17" s="15">
-        <v>0</v>
+        <v>802703.11982014019</v>
       </c>
       <c r="N17" s="15">
-        <v>0</v>
+        <v>204412.67687368783</v>
       </c>
       <c r="O17" s="15">
         <v>0</v>
@@ -2422,28 +2420,28 @@
         <v>42</v>
       </c>
       <c r="E18" s="14">
-        <v>43763.978517646319</v>
+        <v>58933.521905901594</v>
       </c>
       <c r="F18" s="15">
-        <v>1261728.1978450278</v>
+        <v>1243388.8572053353</v>
       </c>
       <c r="G18" s="15">
-        <v>367397.85566209425</v>
+        <v>378882.97400441696</v>
       </c>
       <c r="H18" s="15">
-        <v>4833323.2046840414</v>
+        <v>4286444.7468843479</v>
       </c>
       <c r="I18" s="15">
-        <v>19560.027310772057</v>
+        <v>31109.987250275444</v>
       </c>
       <c r="J18" s="15">
-        <v>857396.56827209215</v>
+        <v>898321.88750478718</v>
       </c>
       <c r="K18" s="15">
-        <v>250974.27487646061</v>
+        <v>271453.90956404991</v>
       </c>
       <c r="L18" s="15">
-        <v>4640128.2654448878</v>
+        <v>4359561.9561253022</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -2459,28 +2457,28 @@
         <v>40</v>
       </c>
       <c r="E19" s="14">
-        <v>0</v>
+        <v>-21879.784508782846</v>
       </c>
       <c r="F19" s="15">
-        <v>0</v>
+        <v>-56645.715326882782</v>
       </c>
       <c r="G19" s="15">
-        <v>0</v>
+        <v>-28584.539119069173</v>
       </c>
       <c r="H19" s="15">
-        <v>0</v>
+        <v>275860.7389547326</v>
       </c>
       <c r="I19" s="15">
-        <v>0</v>
+        <v>-11549.959939503386</v>
       </c>
       <c r="J19" s="15">
-        <v>0</v>
+        <v>-40925.319232695016</v>
       </c>
       <c r="K19" s="15">
-        <v>0</v>
+        <v>-20479.634687589296</v>
       </c>
       <c r="L19" s="15">
-        <v>0</v>
+        <v>280566.30931958527</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -2496,28 +2494,28 @@
         <v>39</v>
       </c>
       <c r="E20" s="14">
-        <v>167517.38477739022</v>
+        <v>164124.41394568497</v>
       </c>
       <c r="F20" s="15">
-        <v>1240315.4284159234</v>
+        <v>1042981.2439283638</v>
       </c>
       <c r="G20" s="15">
-        <v>367285.61832482147</v>
+        <v>354541.724209106</v>
       </c>
       <c r="H20" s="15">
-        <v>3498020.896852497</v>
+        <v>3339665.3179168464</v>
       </c>
       <c r="I20" s="15">
-        <v>92545.603780070684</v>
+        <v>86638.440401741609</v>
       </c>
       <c r="J20" s="15">
-        <v>1062327.7036943426</v>
+        <v>753531.66810879018</v>
       </c>
       <c r="K20" s="15">
-        <v>285441.84035155841</v>
+        <v>254014.41538256884</v>
       </c>
       <c r="L20" s="15">
-        <v>3548107.4336284427</v>
+        <v>3396632.5768608404</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -2552,9 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2824,7 +2820,7 @@
       </c>
       <c r="M12" s="17">
         <f>Use!M8</f>
-        <v>106323.30801193547</v>
+        <v>107505.47667736365</v>
       </c>
       <c r="N12" s="17">
         <f>Use!N8</f>
@@ -2832,7 +2828,7 @@
       </c>
       <c r="O12" s="13">
         <f>Use!O8</f>
-        <v>3644.0177900101125</v>
+        <v>1308.0435919927895</v>
       </c>
       <c r="P12" s="13">
         <f>Use!P8</f>
@@ -2840,7 +2836,7 @@
       </c>
       <c r="Q12" s="13">
         <f>Use!Q8</f>
-        <v>0</v>
+        <v>1153.8055325891473</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -2886,7 +2882,7 @@
       </c>
       <c r="M13" s="19">
         <f>Use!M9</f>
-        <v>2105933.2445719279</v>
+        <v>1474543.7225576744</v>
       </c>
       <c r="N13" s="19">
         <f>Use!N9</f>
@@ -2894,7 +2890,7 @@
       </c>
       <c r="O13" s="15">
         <f>Use!O9</f>
-        <v>208239.87900312577</v>
+        <v>75687.804288948028</v>
       </c>
       <c r="P13" s="15">
         <f>Use!P9</f>
@@ -2902,7 +2898,7 @@
       </c>
       <c r="Q13" s="15">
         <f>Use!Q9</f>
-        <v>0</v>
+        <v>763941.59672843106</v>
       </c>
       <c r="S13" s="1"/>
       <c r="V13" s="1"/>
@@ -2947,7 +2943,7 @@
       </c>
       <c r="M14" s="19">
         <f>Use!M10</f>
-        <v>53676.343922698812</v>
+        <v>51285.594170836637</v>
       </c>
       <c r="N14" s="19">
         <f>Use!N10</f>
@@ -2955,7 +2951,7 @@
       </c>
       <c r="O14" s="15">
         <f>Use!O10</f>
-        <v>33.814618238095967</v>
+        <v>12.6499589841122</v>
       </c>
       <c r="P14" s="15">
         <f>Use!P10</f>
@@ -2963,7 +2959,7 @@
       </c>
       <c r="Q14" s="15">
         <f>Use!Q10</f>
-        <v>0</v>
+        <v>2411.9144111161586</v>
       </c>
       <c r="S14" s="1"/>
       <c r="V14" s="1"/>
@@ -3008,7 +3004,7 @@
       </c>
       <c r="M15" s="19">
         <f>Use!M11</f>
-        <v>7048312.6373048685</v>
+        <v>6870975.4274285519</v>
       </c>
       <c r="N15" s="19">
         <f>Use!N11</f>
@@ -3016,7 +3012,7 @@
       </c>
       <c r="O15" s="15">
         <f>Use!O11</f>
-        <v>106436.84578341726</v>
+        <v>49187.589449195468</v>
       </c>
       <c r="P15" s="15">
         <f>Use!P11</f>
@@ -3024,7 +3020,7 @@
       </c>
       <c r="Q15" s="15">
         <f>Use!Q11</f>
-        <v>0</v>
+        <v>234586.46621053852</v>
       </c>
       <c r="S15" s="1"/>
       <c r="V15" s="1"/>
@@ -3077,7 +3073,7 @@
       </c>
       <c r="O16" s="19">
         <f>Use!O12</f>
-        <v>48683.249698980326</v>
+        <v>40502.66470631156</v>
       </c>
       <c r="P16" s="19">
         <f>Use!P12</f>
@@ -3085,7 +3081,7 @@
       </c>
       <c r="Q16" s="15">
         <f>Use!Q12</f>
-        <v>0</v>
+        <v>8180.5849926687661</v>
       </c>
       <c r="S16" s="1"/>
       <c r="V16" s="1"/>
@@ -3138,7 +3134,7 @@
       </c>
       <c r="O17" s="19">
         <f>Use!O13</f>
-        <v>1149202.8091295597</v>
+        <v>1075890.5722947831</v>
       </c>
       <c r="P17" s="19">
         <f>Use!P13</f>
@@ -3146,7 +3142,7 @@
       </c>
       <c r="Q17" s="15">
         <f>Use!Q13</f>
-        <v>0</v>
+        <v>73312.236834776588</v>
       </c>
       <c r="S17" s="1"/>
       <c r="V17" s="1"/>
@@ -3199,7 +3195,7 @@
       </c>
       <c r="O18" s="19">
         <f>Use!O14</f>
-        <v>45.404385260888375</v>
+        <v>0</v>
       </c>
       <c r="P18" s="19">
         <f>Use!P14</f>
@@ -3207,7 +3203,7 @@
       </c>
       <c r="Q18" s="15">
         <f>Use!Q14</f>
-        <v>0</v>
+        <v>45.404385260888375</v>
       </c>
       <c r="S18" s="1"/>
       <c r="V18" s="1"/>
@@ -3260,7 +3256,7 @@
       </c>
       <c r="O19" s="19">
         <f>Use!O15</f>
-        <v>7378638.9453427522</v>
+        <v>7260288.2363079153</v>
       </c>
       <c r="P19" s="19">
         <f>Use!P15</f>
@@ -3268,7 +3264,7 @@
       </c>
       <c r="Q19" s="15">
         <f>Use!Q15</f>
-        <v>0</v>
+        <v>118350.70903483592</v>
       </c>
       <c r="S19" s="1"/>
       <c r="V19" s="1"/>
@@ -3283,44 +3279,44 @@
       </c>
       <c r="E20" s="14">
         <f t="array" ref="E20:L24">MMULT(Additional_calculatations!D133:K137,MMULT(Additional_calculatations!P66:W73,Additional_calculatations!D24:K31))</f>
-        <v>0</v>
+        <v>2862.4017257827195</v>
       </c>
       <c r="F20" s="15">
-        <v>0</v>
+        <v>196738.65514534444</v>
       </c>
       <c r="G20" s="15">
-        <v>0</v>
+        <v>12439.588982340463</v>
       </c>
       <c r="H20" s="15">
-        <v>0</v>
+        <v>159785.98595963256</v>
       </c>
       <c r="I20" s="15">
-        <v>0</v>
+        <v>5936.2933445240051</v>
       </c>
       <c r="J20" s="15">
-        <v>0</v>
+        <v>314554.82069407601</v>
       </c>
       <c r="K20" s="15">
-        <v>0</v>
+        <v>31427.424968989566</v>
       </c>
       <c r="L20" s="15">
-        <v>0</v>
+        <v>145686.94169288382</v>
       </c>
       <c r="M20" s="15">
         <f>Use!M16</f>
-        <v>0</v>
+        <v>153449.63972739296</v>
       </c>
       <c r="N20" s="15">
         <f>Use!N16</f>
-        <v>0</v>
+        <v>86963.012198008553</v>
       </c>
       <c r="O20" s="15">
         <f>Use!O16</f>
-        <v>0</v>
+        <v>3520149.4394018687</v>
       </c>
       <c r="P20" s="15">
         <f>Use!P16</f>
-        <v>0</v>
+        <v>989188.49839271954</v>
       </c>
       <c r="Q20" s="1"/>
     </row>
@@ -3332,16 +3328,16 @@
         <v>41</v>
       </c>
       <c r="E21" s="14">
-        <v>0</v>
+        <v>6428.4694215280615</v>
       </c>
       <c r="F21" s="15">
-        <v>0</v>
+        <v>69047.835150826533</v>
       </c>
       <c r="G21" s="15">
-        <v>0</v>
+        <v>16862.592684930412</v>
       </c>
       <c r="H21" s="15">
-        <v>0</v>
+        <v>277473.53945152601</v>
       </c>
       <c r="I21" s="15">
         <v>0</v>
@@ -3357,11 +3353,11 @@
       </c>
       <c r="M21" s="15">
         <f>Use!M17</f>
-        <v>0</v>
+        <v>802703.11982014019</v>
       </c>
       <c r="N21" s="15">
         <f>Use!N17</f>
-        <v>0</v>
+        <v>204412.67687368783</v>
       </c>
       <c r="O21" s="15">
         <f>Use!O17</f>
@@ -3381,28 +3377,28 @@
         <v>42</v>
       </c>
       <c r="E22" s="14">
-        <v>38005.088619822549</v>
+        <v>53711.037912679749</v>
       </c>
       <c r="F22" s="15">
-        <v>1154052.8246036423</v>
+        <v>1149535.787908897</v>
       </c>
       <c r="G22" s="15">
-        <v>365559.83363560599</v>
+        <v>378923.61231456313</v>
       </c>
       <c r="H22" s="15">
-        <v>4948595.4898497388</v>
+        <v>4385479.6618638616</v>
       </c>
       <c r="I22" s="15">
-        <v>19289.599133732048</v>
+        <v>30947.709772258451</v>
       </c>
       <c r="J22" s="15">
-        <v>833622.73669643328</v>
+        <v>878145.16797836684</v>
       </c>
       <c r="K22" s="15">
-        <v>250974.27487646061</v>
+        <v>271453.90956404991</v>
       </c>
       <c r="L22" s="15">
-        <v>4664172.5251975879</v>
+        <v>4379900.9531297395</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -3418,28 +3414,28 @@
         <v>40</v>
       </c>
       <c r="E23" s="14">
-        <v>0</v>
+        <v>-22134.418714385258</v>
       </c>
       <c r="F23" s="15">
-        <v>0</v>
+        <v>-64530.798456081058</v>
       </c>
       <c r="G23" s="15">
-        <v>0</v>
+        <v>-30226.371363887447</v>
       </c>
       <c r="H23" s="15">
-        <v>0</v>
+        <v>285642.28853435145</v>
       </c>
       <c r="I23" s="15">
-        <v>0</v>
+        <v>-11658.110638526397</v>
       </c>
       <c r="J23" s="15">
-        <v>0</v>
+        <v>-44522.431281933445</v>
       </c>
       <c r="K23" s="15">
-        <v>0</v>
+        <v>-20479.634687589296</v>
       </c>
       <c r="L23" s="15">
-        <v>0</v>
+        <v>284271.57206784672</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -3455,28 +3451,28 @@
         <v>39</v>
       </c>
       <c r="E24" s="14">
-        <v>164011.64664549727</v>
+        <v>161149.2454421006</v>
       </c>
       <c r="F24" s="15">
-        <v>1166743.1904560106</v>
+        <v>970004.53638034139</v>
       </c>
       <c r="G24" s="15">
-        <v>368958.07749031053</v>
+        <v>356518.48850107449</v>
       </c>
       <c r="H24" s="15">
-        <v>3573426.4137788131</v>
+        <v>3413640.4296764848</v>
       </c>
       <c r="I24" s="15">
-        <v>92898.232825536776</v>
+        <v>86961.939481012771</v>
       </c>
       <c r="J24" s="15">
-        <v>1053618.5652984329</v>
+        <v>739063.74460435682</v>
       </c>
       <c r="K24" s="15">
-        <v>285441.84035155841</v>
+        <v>254014.41538256884</v>
       </c>
       <c r="L24" s="15">
-        <v>3556463.9429788864</v>
+        <v>3410777.0012860033</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -3597,19 +3593,19 @@
       </c>
       <c r="E31" s="40">
         <f>E12/SUM(E$12:E$24)</f>
-        <v>0.13560568481534296</v>
+        <v>0.13560568464641432</v>
       </c>
       <c r="F31" s="41">
         <f t="shared" ref="F31:L31" si="0">F12/SUM(F$12:F$24)</f>
-        <v>2.6850134634168493E-2</v>
+        <v>2.6850134630243851E-2</v>
       </c>
       <c r="G31" s="41">
         <f t="shared" si="0"/>
-        <v>1.3530475854401213E-3</v>
+        <v>1.3530475854452051E-3</v>
       </c>
       <c r="H31" s="41">
         <f t="shared" si="0"/>
-        <v>1.7884261461248428E-3</v>
+        <v>1.788426145885802E-3</v>
       </c>
       <c r="I31" s="42">
         <f t="shared" si="0"/>
@@ -3640,19 +3636,19 @@
       </c>
       <c r="E32" s="43">
         <f t="shared" ref="E32:L32" si="1">E13/SUM(E$12:E$24)</f>
-        <v>0.20315259019055831</v>
+        <v>0.2031525899374842</v>
       </c>
       <c r="F32" s="44">
         <f t="shared" si="1"/>
-        <v>0.37773486179894294</v>
+        <v>0.37773486174373</v>
       </c>
       <c r="G32" s="44">
         <f t="shared" si="1"/>
-        <v>0.21444584230872152</v>
+        <v>0.21444584230952723</v>
       </c>
       <c r="H32" s="44">
         <f t="shared" si="1"/>
-        <v>6.3748888088665315E-2</v>
+        <v>6.3748888080144644E-2</v>
       </c>
       <c r="I32" s="38">
         <f t="shared" si="1"/>
@@ -3683,19 +3679,19 @@
       </c>
       <c r="E33" s="43">
         <f t="shared" ref="E33:L33" si="2">E14/SUM(E$12:E$24)</f>
-        <v>5.3130454035925905E-3</v>
+        <v>5.3130453969739483E-3</v>
       </c>
       <c r="F33" s="44">
         <f t="shared" si="2"/>
-        <v>4.9687362331358349E-3</v>
+        <v>4.9687362324095626E-3</v>
       </c>
       <c r="G33" s="44">
         <f t="shared" si="2"/>
-        <v>0.19875545949601922</v>
+        <v>0.19875545949676601</v>
       </c>
       <c r="H33" s="44">
         <f t="shared" si="2"/>
-        <v>1.4048326384615971E-2</v>
+        <v>1.4048326382738272E-2</v>
       </c>
       <c r="I33" s="38">
         <f t="shared" si="2"/>
@@ -3726,19 +3722,19 @@
       </c>
       <c r="E34" s="43">
         <f t="shared" ref="E34:L34" si="3">E15/SUM(E$12:E$24)</f>
-        <v>0.1560649998005583</v>
+        <v>0.15606499960614278</v>
       </c>
       <c r="F34" s="44">
         <f t="shared" si="3"/>
-        <v>0.20094571822005727</v>
+        <v>0.20094571819068532</v>
       </c>
       <c r="G34" s="44">
         <f t="shared" si="3"/>
-        <v>0.1699881416890669</v>
+        <v>0.16998814168970558</v>
       </c>
       <c r="H34" s="44">
         <f t="shared" si="3"/>
-        <v>0.29901701144639253</v>
+        <v>0.29901701140642595</v>
       </c>
       <c r="I34" s="38">
         <f t="shared" si="3"/>
@@ -3769,19 +3765,19 @@
       </c>
       <c r="E35" s="37">
         <f t="shared" ref="E35:L35" si="4">E16/SUM(E$12:E$24)</f>
-        <v>3.6707293877734884E-3</v>
+        <v>3.6707293832007352E-3</v>
       </c>
       <c r="F35" s="38">
         <f t="shared" si="4"/>
-        <v>1.3295327085813629E-3</v>
+        <v>1.329532708387027E-3</v>
       </c>
       <c r="G35" s="38">
         <f t="shared" si="4"/>
-        <v>3.9653227352474427E-5</v>
+        <v>3.9653227352623416E-5</v>
       </c>
       <c r="H35" s="38">
         <f t="shared" si="4"/>
-        <v>6.5259870198072583E-5</v>
+        <v>6.5259870189349946E-5</v>
       </c>
       <c r="I35" s="44">
         <f t="shared" si="4"/>
@@ -3812,19 +3808,19 @@
       </c>
       <c r="E36" s="37">
         <f t="shared" ref="E36:L36" si="5">E17/SUM(E$12:E$24)</f>
-        <v>7.8483543483332443E-3</v>
+        <v>7.8483543385562821E-3</v>
       </c>
       <c r="F36" s="38">
         <f t="shared" si="5"/>
-        <v>4.4820292903533343E-2</v>
+        <v>4.4820292896982028E-2</v>
       </c>
       <c r="G36" s="38">
         <f t="shared" si="5"/>
-        <v>8.9365765309115369E-3</v>
+        <v>8.9365765309451142E-3</v>
       </c>
       <c r="H36" s="38">
         <f t="shared" si="5"/>
-        <v>4.1458900183826272E-3</v>
+        <v>4.1458900178284871E-3</v>
       </c>
       <c r="I36" s="44">
         <f t="shared" si="5"/>
@@ -3898,19 +3894,19 @@
       </c>
       <c r="E38" s="37">
         <f t="shared" ref="E38:L38" si="7">E19/SUM(E$12:E$24)</f>
-        <v>6.5952367638117109E-3</v>
+        <v>6.5952367555957995E-3</v>
       </c>
       <c r="F38" s="38">
         <f t="shared" si="7"/>
-        <v>2.6219581252632282E-2</v>
+        <v>2.6219581248799806E-2</v>
       </c>
       <c r="G38" s="38">
         <f t="shared" si="7"/>
-        <v>6.2636223091100977E-3</v>
+        <v>6.2636223091336327E-3</v>
       </c>
       <c r="H38" s="38">
         <f t="shared" si="7"/>
-        <v>3.902339597468388E-3</v>
+        <v>3.9023395969468013E-3</v>
       </c>
       <c r="I38" s="44">
         <f t="shared" si="7"/>
@@ -4037,28 +4033,28 @@
       </c>
       <c r="E46" s="40">
         <f t="array" ref="E46:L53">MINVERSE(Additional_calculatations!D144:K151-ModelA_product_technology!E31:L38)</f>
-        <v>1.171323557533092</v>
+        <v>1.1713235572792624</v>
       </c>
       <c r="F46" s="41">
-        <v>5.4012342631205766E-2</v>
+        <v>5.4012342605762868E-2</v>
       </c>
       <c r="G46" s="41">
-        <v>1.8295318612581553E-2</v>
+        <v>1.8295318604393627E-2</v>
       </c>
       <c r="H46" s="41">
-        <v>8.3202663262811078E-3</v>
+        <v>8.3202663215513895E-3</v>
       </c>
       <c r="I46" s="42">
-        <v>1.3275311442996896E-2</v>
+        <v>1.3275311439701841E-2</v>
       </c>
       <c r="J46" s="42">
-        <v>7.9325590380791757E-3</v>
+        <v>7.9325590354587094E-3</v>
       </c>
       <c r="K46" s="42">
-        <v>2.9310495951179361E-3</v>
+        <v>2.9310495940021069E-3</v>
       </c>
       <c r="L46" s="42">
-        <v>9.0720543013290489E-4</v>
+        <v>9.0720542978825675E-4</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -4072,28 +4068,28 @@
         <v>8</v>
       </c>
       <c r="E47" s="43">
-        <v>0.43167138096260965</v>
+        <v>0.43167138028049873</v>
       </c>
       <c r="F47" s="44">
-        <v>1.6913205252211707</v>
+        <v>1.691320525010042</v>
       </c>
       <c r="G47" s="44">
-        <v>0.48978904132175788</v>
+        <v>0.48978904125474249</v>
       </c>
       <c r="H47" s="44">
-        <v>0.16544088472009358</v>
+        <v>0.16544088466614876</v>
       </c>
       <c r="I47" s="38">
-        <v>5.1955353723153311E-2</v>
+        <v>5.1955353709739006E-2</v>
       </c>
       <c r="J47" s="38">
-        <v>0.10516019285858418</v>
+        <v>0.10516019284175963</v>
       </c>
       <c r="K47" s="38">
-        <v>5.4118510352913242E-2</v>
+        <v>5.411851034461615E-2</v>
       </c>
       <c r="L47" s="38">
-        <v>1.520652528761382E-2</v>
+        <v>1.5206525284973745E-2</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -4107,28 +4103,28 @@
         <v>9</v>
       </c>
       <c r="E48" s="43">
-        <v>1.7303888956534733E-2</v>
+        <v>1.7303888928640845E-2</v>
       </c>
       <c r="F48" s="44">
-        <v>1.9744577503674584E-2</v>
+        <v>1.9744577495812068E-2</v>
       </c>
       <c r="G48" s="44">
-        <v>1.2591502316530887</v>
+        <v>1.2591502316508691</v>
       </c>
       <c r="H48" s="44">
-        <v>2.7091434937588227E-2</v>
+        <v>2.7091434931586219E-2</v>
       </c>
       <c r="I48" s="38">
-        <v>1.6817827671633653E-3</v>
+        <v>1.6817827665604598E-3</v>
       </c>
       <c r="J48" s="38">
-        <v>2.3026325974264805E-3</v>
+        <v>2.3026325966370815E-3</v>
       </c>
       <c r="K48" s="38">
-        <v>1.4303696486466172E-3</v>
+        <v>1.4303696482231415E-3</v>
       </c>
       <c r="L48" s="38">
-        <v>6.1086475517345797E-4</v>
+        <v>6.1086475500961616E-4</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -4142,28 +4138,28 @@
         <v>10</v>
       </c>
       <c r="E49" s="43">
-        <v>0.39099634664078814</v>
+        <v>0.3909963460130314</v>
       </c>
       <c r="F49" s="44">
-        <v>0.50710250538414947</v>
+        <v>0.50710250519974365</v>
       </c>
       <c r="G49" s="44">
-        <v>0.45229502855241366</v>
+        <v>0.45229502848011272</v>
       </c>
       <c r="H49" s="44">
-        <v>1.4834246888300529</v>
+        <v>1.4834246887179319</v>
       </c>
       <c r="I49" s="38">
-        <v>4.651561223356588E-2</v>
+        <v>4.6515612220246E-2</v>
       </c>
       <c r="J49" s="38">
-        <v>8.7585318009347407E-2</v>
+        <v>8.7585317992033535E-2</v>
       </c>
       <c r="K49" s="38">
-        <v>5.6751146450305677E-2</v>
+        <v>5.6751146441202084E-2</v>
       </c>
       <c r="L49" s="38">
-        <v>2.7890918060169186E-2</v>
+        <v>2.7890918056799035E-2</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -4177,28 +4173,28 @@
         <v>7</v>
       </c>
       <c r="E50" s="37">
-        <v>7.855960192006569E-3</v>
+        <v>7.8559601799976075E-3</v>
       </c>
       <c r="F50" s="38">
-        <v>7.6229334727653539E-3</v>
+        <v>7.622933470268046E-3</v>
       </c>
       <c r="G50" s="38">
-        <v>3.0363343767275935E-3</v>
+        <v>3.0363343759418774E-3</v>
       </c>
       <c r="H50" s="38">
-        <v>1.245515845403636E-3</v>
+        <v>1.2455158448912255E-3</v>
       </c>
       <c r="I50" s="44">
-        <v>1.2432407029510144</v>
+        <v>1.243240702950819</v>
       </c>
       <c r="J50" s="44">
-        <v>5.5367478684414072E-2</v>
+        <v>5.5367478684204725E-2</v>
       </c>
       <c r="K50" s="44">
-        <v>1.4403464601579432E-2</v>
+        <v>1.4403464601481012E-2</v>
       </c>
       <c r="L50" s="44">
-        <v>5.0599034703171309E-3</v>
+        <v>5.0599034702866726E-3</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -4212,28 +4208,28 @@
         <v>8</v>
       </c>
       <c r="E51" s="37">
-        <v>4.9532746355485949E-2</v>
+        <v>4.9532746274269117E-2</v>
       </c>
       <c r="F51" s="38">
-        <v>0.12349601082749605</v>
+        <v>0.12349601079214266</v>
       </c>
       <c r="G51" s="38">
-        <v>5.548776834938899E-2</v>
+        <v>5.5487768338348516E-2</v>
       </c>
       <c r="H51" s="38">
-        <v>2.2046647713318518E-2</v>
+        <v>2.204664770545307E-2</v>
       </c>
       <c r="I51" s="44">
-        <v>0.38975194333248625</v>
+        <v>0.38975194333059271</v>
       </c>
       <c r="J51" s="44">
-        <v>1.4947002281483228</v>
+        <v>1.4947002281456778</v>
       </c>
       <c r="K51" s="44">
-        <v>0.35821600493842881</v>
+        <v>0.35821600493710409</v>
       </c>
       <c r="L51" s="44">
-        <v>0.12587263598667667</v>
+        <v>0.12587263598626416</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -4247,28 +4243,28 @@
         <v>9</v>
       </c>
       <c r="E52" s="37">
-        <v>6.8817366528824055E-4</v>
+        <v>6.8817366416901724E-4</v>
       </c>
       <c r="F52" s="38">
-        <v>1.5726121827208974E-3</v>
+        <v>1.5726121822652621E-3</v>
       </c>
       <c r="G52" s="38">
-        <v>7.2296607396181531E-4</v>
+        <v>7.2296607381858483E-4</v>
       </c>
       <c r="H52" s="38">
-        <v>3.0404745745406584E-4</v>
+        <v>3.0404745734869244E-4</v>
       </c>
       <c r="I52" s="44">
-        <v>1.1933469815397821E-2</v>
+        <v>1.1933469815372612E-2</v>
       </c>
       <c r="J52" s="44">
-        <v>1.195798123772975E-2</v>
+        <v>1.1957981237695229E-2</v>
       </c>
       <c r="K52" s="44">
-        <v>1.0062876330575996</v>
+        <v>1.0062876330575823</v>
       </c>
       <c r="L52" s="44">
-        <v>1.3104280951235928E-2</v>
+        <v>1.3104280951230523E-2</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -4282,28 +4278,28 @@
         <v>10</v>
       </c>
       <c r="E53" s="37">
-        <v>4.378765948773742E-2</v>
+        <v>4.378765941646505E-2</v>
       </c>
       <c r="F53" s="38">
-        <v>9.9907388492209398E-2</v>
+        <v>9.9907388463169031E-2</v>
       </c>
       <c r="G53" s="38">
-        <v>4.7050799391721271E-2</v>
+        <v>4.7050799382545791E-2</v>
       </c>
       <c r="H53" s="38">
-        <v>2.0636676959602727E-2</v>
+        <v>2.0636676952645944E-2</v>
       </c>
       <c r="I53" s="44">
-        <v>0.367354972608393</v>
+        <v>0.36735497260678213</v>
       </c>
       <c r="J53" s="44">
-        <v>0.40375462121584199</v>
+        <v>0.40375462121363243</v>
       </c>
       <c r="K53" s="44">
-        <v>0.41151372750320209</v>
+        <v>0.41151372750209564</v>
       </c>
       <c r="L53" s="44">
-        <v>1.4503562916430015</v>
+        <v>1.4503562916426531</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4404,35 +4400,35 @@
       <c r="D60" s="65"/>
       <c r="E60" s="45">
         <f>SUM(E46:E53)</f>
-        <v>2.1131597137935425</v>
+        <v>2.1131597120363339</v>
       </c>
       <c r="F60" s="46">
         <f t="shared" ref="F60:L60" si="8">SUM(F46:F53)</f>
-        <v>2.5047788957153925</v>
+        <v>2.5047788952192058</v>
       </c>
       <c r="G60" s="46">
         <f t="shared" si="8"/>
-        <v>2.3258274883316412</v>
+        <v>2.3258274881607726</v>
       </c>
       <c r="H60" s="46">
         <f t="shared" si="8"/>
-        <v>1.7285101627897947</v>
+        <v>1.7285101625975574</v>
       </c>
       <c r="I60" s="46">
         <f t="shared" si="8"/>
-        <v>2.1257091488741708</v>
+        <v>2.1257091488398139</v>
       </c>
       <c r="J60" s="46">
         <f t="shared" si="8"/>
-        <v>2.1687610117897456</v>
+        <v>2.1687610117470992</v>
       </c>
       <c r="K60" s="46">
         <f t="shared" si="8"/>
-        <v>1.9056519061477935</v>
+        <v>1.9056519061263066</v>
       </c>
       <c r="L60" s="46">
         <f t="shared" si="8"/>
-        <v>1.6390086255843206</v>
+        <v>1.6390086255770051</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4442,35 +4438,35 @@
       <c r="D61" s="67"/>
       <c r="E61" s="47">
         <f>SUMIF($B$46:$B$53,E$57,E46:E53)</f>
-        <v>2.0112951740930245</v>
+        <v>2.0112951725014332</v>
       </c>
       <c r="F61" s="48">
         <f t="shared" ref="F61:L61" si="9">SUMIF($B$46:$B$53,F$57,F46:F53)</f>
-        <v>2.2721799507402007</v>
+        <v>2.2721799503113607</v>
       </c>
       <c r="G61" s="48">
         <f t="shared" si="9"/>
-        <v>2.2195296201398418</v>
+        <v>2.219529619990118</v>
       </c>
       <c r="H61" s="48">
         <f t="shared" si="9"/>
-        <v>1.6842772748140158</v>
+        <v>1.6842772746372183</v>
       </c>
       <c r="I61" s="48">
         <f t="shared" si="9"/>
-        <v>2.0122810887072915</v>
+        <v>2.0122810887035665</v>
       </c>
       <c r="J61" s="48">
         <f t="shared" si="9"/>
-        <v>1.9657803092863086</v>
+        <v>1.9657803092812103</v>
       </c>
       <c r="K61" s="48">
         <f t="shared" si="9"/>
-        <v>1.79042083010081</v>
+        <v>1.7904208300982631</v>
       </c>
       <c r="L61" s="48">
         <f t="shared" si="9"/>
-        <v>1.5943931120512311</v>
+        <v>1.5943931120504344</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4480,35 +4476,35 @@
       <c r="D62" s="67"/>
       <c r="E62" s="47">
         <f>SUM(E46:E53)-E61</f>
-        <v>0.10186453970051801</v>
+        <v>0.10186453953490071</v>
       </c>
       <c r="F62" s="48">
         <f t="shared" ref="F62:L62" si="10">SUM(F46:F53)-F61</f>
-        <v>0.23259894497519173</v>
+        <v>0.23259894490784516</v>
       </c>
       <c r="G62" s="48">
         <f t="shared" si="10"/>
-        <v>0.10629786819179943</v>
+        <v>0.10629786817065456</v>
       </c>
       <c r="H62" s="48">
         <f t="shared" si="10"/>
-        <v>4.4232887975778956E-2</v>
+        <v>4.4232887960339085E-2</v>
       </c>
       <c r="I62" s="48">
         <f t="shared" si="10"/>
-        <v>0.11342806016687934</v>
+        <v>0.1134280601362474</v>
       </c>
       <c r="J62" s="48">
         <f t="shared" si="10"/>
-        <v>0.20298070250343692</v>
+        <v>0.20298070246588895</v>
       </c>
       <c r="K62" s="48">
         <f t="shared" si="10"/>
-        <v>0.11523107604698346</v>
+        <v>0.1152310760280435</v>
       </c>
       <c r="L62" s="48">
         <f t="shared" si="10"/>
-        <v>4.4615513533089457E-2</v>
+        <v>4.4615513526570671E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4537,9 +4533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4809,7 +4803,7 @@
       </c>
       <c r="M12" s="17">
         <f>Use!M8</f>
-        <v>106323.30801193547</v>
+        <v>107505.47667736365</v>
       </c>
       <c r="N12" s="17">
         <f>Use!N8</f>
@@ -4817,7 +4811,7 @@
       </c>
       <c r="O12" s="13">
         <f>Use!O8</f>
-        <v>3644.0177900101125</v>
+        <v>1308.0435919927895</v>
       </c>
       <c r="P12" s="13">
         <f>Use!P8</f>
@@ -4825,7 +4819,7 @@
       </c>
       <c r="Q12" s="13">
         <f>Use!Q8</f>
-        <v>0</v>
+        <v>1153.8055325891473</v>
       </c>
       <c r="S12" s="1"/>
       <c r="V12" s="1"/>
@@ -4870,7 +4864,7 @@
       </c>
       <c r="M13" s="19">
         <f>Use!M9</f>
-        <v>2105933.2445719279</v>
+        <v>1474543.7225576744</v>
       </c>
       <c r="N13" s="19">
         <f>Use!N9</f>
@@ -4878,7 +4872,7 @@
       </c>
       <c r="O13" s="15">
         <f>Use!O9</f>
-        <v>208239.87900312577</v>
+        <v>75687.804288948028</v>
       </c>
       <c r="P13" s="15">
         <f>Use!P9</f>
@@ -4886,7 +4880,7 @@
       </c>
       <c r="Q13" s="15">
         <f>Use!Q9</f>
-        <v>0</v>
+        <v>763941.59672843106</v>
       </c>
       <c r="S13" s="1"/>
       <c r="V13" s="1"/>
@@ -4931,7 +4925,7 @@
       </c>
       <c r="M14" s="19">
         <f>Use!M10</f>
-        <v>53676.343922698812</v>
+        <v>51285.594170836637</v>
       </c>
       <c r="N14" s="19">
         <f>Use!N10</f>
@@ -4939,7 +4933,7 @@
       </c>
       <c r="O14" s="15">
         <f>Use!O10</f>
-        <v>33.814618238095967</v>
+        <v>12.6499589841122</v>
       </c>
       <c r="P14" s="15">
         <f>Use!P10</f>
@@ -4947,7 +4941,7 @@
       </c>
       <c r="Q14" s="15">
         <f>Use!Q10</f>
-        <v>0</v>
+        <v>2411.9144111161586</v>
       </c>
       <c r="S14" s="1"/>
       <c r="V14" s="1"/>
@@ -4992,7 +4986,7 @@
       </c>
       <c r="M15" s="19">
         <f>Use!M11</f>
-        <v>7048312.6373048685</v>
+        <v>6870975.4274285519</v>
       </c>
       <c r="N15" s="19">
         <f>Use!N11</f>
@@ -5000,7 +4994,7 @@
       </c>
       <c r="O15" s="15">
         <f>Use!O11</f>
-        <v>106436.84578341726</v>
+        <v>49187.589449195468</v>
       </c>
       <c r="P15" s="15">
         <f>Use!P11</f>
@@ -5008,7 +5002,7 @@
       </c>
       <c r="Q15" s="15">
         <f>Use!Q11</f>
-        <v>0</v>
+        <v>234586.46621053852</v>
       </c>
       <c r="S15" s="1"/>
       <c r="V15" s="1"/>
@@ -5061,7 +5055,7 @@
       </c>
       <c r="O16" s="19">
         <f>Use!O12</f>
-        <v>48683.249698980326</v>
+        <v>40502.66470631156</v>
       </c>
       <c r="P16" s="19">
         <f>Use!P12</f>
@@ -5069,7 +5063,7 @@
       </c>
       <c r="Q16" s="15">
         <f>Use!Q12</f>
-        <v>0</v>
+        <v>8180.5849926687661</v>
       </c>
       <c r="S16" s="1"/>
       <c r="V16" s="1"/>
@@ -5122,7 +5116,7 @@
       </c>
       <c r="O17" s="19">
         <f>Use!O13</f>
-        <v>1149202.8091295597</v>
+        <v>1075890.5722947831</v>
       </c>
       <c r="P17" s="19">
         <f>Use!P13</f>
@@ -5130,7 +5124,7 @@
       </c>
       <c r="Q17" s="15">
         <f>Use!Q13</f>
-        <v>0</v>
+        <v>73312.236834776588</v>
       </c>
       <c r="S17" s="1"/>
       <c r="V17" s="1"/>
@@ -5183,7 +5177,7 @@
       </c>
       <c r="O18" s="19">
         <f>Use!O14</f>
-        <v>45.404385260888375</v>
+        <v>0</v>
       </c>
       <c r="P18" s="19">
         <f>Use!P14</f>
@@ -5191,7 +5185,7 @@
       </c>
       <c r="Q18" s="15">
         <f>Use!Q14</f>
-        <v>0</v>
+        <v>45.404385260888375</v>
       </c>
       <c r="S18" s="1"/>
       <c r="V18" s="1"/>
@@ -5244,7 +5238,7 @@
       </c>
       <c r="O19" s="19">
         <f>Use!O15</f>
-        <v>7378638.9453427522</v>
+        <v>7260288.2363079153</v>
       </c>
       <c r="P19" s="19">
         <f>Use!P15</f>
@@ -5252,7 +5246,7 @@
       </c>
       <c r="Q19" s="15">
         <f>Use!Q15</f>
-        <v>0</v>
+        <v>118350.70903483592</v>
       </c>
       <c r="S19" s="1"/>
       <c r="V19" s="1"/>
@@ -5267,44 +5261,44 @@
       </c>
       <c r="E20" s="14">
         <f t="array" ref="E20:L24">MMULT(Additional_calculatations!D133:K137,MMULT(Additional_calculatations!D80:K87,Additional_calculatations!D24:K31))</f>
-        <v>0</v>
+        <v>3265.1597551204018</v>
       </c>
       <c r="F20" s="15">
-        <v>0</v>
+        <v>189038.81587758247</v>
       </c>
       <c r="G20" s="15">
-        <v>0</v>
+        <v>13445.725576439369</v>
       </c>
       <c r="H20" s="15">
-        <v>0</v>
+        <v>166076.93060395794</v>
       </c>
       <c r="I20" s="15">
-        <v>0</v>
+        <v>5901.8043156442382</v>
       </c>
       <c r="J20" s="15">
-        <v>0</v>
+        <v>301919.64291763195</v>
       </c>
       <c r="K20" s="15">
-        <v>0</v>
+        <v>31427.424968989566</v>
       </c>
       <c r="L20" s="15">
-        <v>0</v>
+        <v>158356.60849820756</v>
       </c>
       <c r="M20" s="15">
         <f>Use!M16</f>
-        <v>0</v>
+        <v>153449.63972739296</v>
       </c>
       <c r="N20" s="15">
         <f>Use!N16</f>
-        <v>0</v>
+        <v>86963.012198008553</v>
       </c>
       <c r="O20" s="15">
         <f>Use!O16</f>
-        <v>0</v>
+        <v>3520149.4394018687</v>
       </c>
       <c r="P20" s="15">
         <f>Use!P16</f>
-        <v>0</v>
+        <v>989188.49839271954</v>
       </c>
       <c r="Q20" s="1"/>
     </row>
@@ -5316,16 +5310,16 @@
         <v>41</v>
       </c>
       <c r="E21" s="14">
-        <v>0</v>
+        <v>6364.9995347199019</v>
       </c>
       <c r="F21" s="15">
-        <v>0</v>
+        <v>73726.700810914001</v>
       </c>
       <c r="G21" s="15">
-        <v>0</v>
+        <v>17687.08243393102</v>
       </c>
       <c r="H21" s="15">
-        <v>0</v>
+        <v>272033.65392924612</v>
       </c>
       <c r="I21" s="15">
         <v>0</v>
@@ -5341,11 +5335,11 @@
       </c>
       <c r="M21" s="15">
         <f>Use!M17</f>
-        <v>0</v>
+        <v>802703.11982014019</v>
       </c>
       <c r="N21" s="15">
         <f>Use!N17</f>
-        <v>0</v>
+        <v>204412.67687368783</v>
       </c>
       <c r="O21" s="15">
         <f>Use!O17</f>
@@ -5365,28 +5359,28 @@
         <v>42</v>
       </c>
       <c r="E22" s="14">
-        <v>42293.600557453719</v>
+        <v>56421.085384677295</v>
       </c>
       <c r="F22" s="15">
-        <v>1240572.9304418322</v>
+        <v>1219613.6355786833</v>
       </c>
       <c r="G22" s="15">
-        <v>375739.2648560151</v>
+        <v>385329.69664421387</v>
       </c>
       <c r="H22" s="15">
-        <v>4847607.4408535073</v>
+        <v>4306285.6823924268</v>
       </c>
       <c r="I22" s="15">
-        <v>20122.882151971229</v>
+        <v>31581.453156555057</v>
       </c>
       <c r="J22" s="15">
-        <v>871434.20268275857</v>
+        <v>909088.05292589113</v>
       </c>
       <c r="K22" s="15">
-        <v>250974.27487646061</v>
+        <v>271453.90956404991</v>
       </c>
       <c r="L22" s="15">
-        <v>4625527.7761930227</v>
+        <v>4348324.324797919</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -5402,28 +5396,28 @@
         <v>40</v>
       </c>
       <c r="E23" s="14">
-        <v>0</v>
+        <v>-20492.484361943472</v>
       </c>
       <c r="F23" s="15">
-        <v>0</v>
+        <v>-52767.40594776487</v>
       </c>
       <c r="G23" s="15">
-        <v>0</v>
+        <v>-27277.514222129779</v>
       </c>
       <c r="H23" s="15">
-        <v>0</v>
+        <v>269288.10453183588</v>
       </c>
       <c r="I23" s="15">
-        <v>0</v>
+        <v>-11458.571004583828</v>
       </c>
       <c r="J23" s="15">
-        <v>0</v>
+        <v>-37653.850243132474</v>
       </c>
       <c r="K23" s="15">
-        <v>0</v>
+        <v>-20479.634687589296</v>
       </c>
       <c r="L23" s="15">
-        <v>0</v>
+        <v>277203.45139510318</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -5439,28 +5433,28 @@
         <v>39</v>
       </c>
       <c r="E24" s="14">
-        <v>158135.61912817074</v>
+        <v>154870.45986168753</v>
       </c>
       <c r="F24" s="15">
-        <v>1214682.8005953252</v>
+        <v>1025643.9857963724</v>
       </c>
       <c r="G24" s="15">
-        <v>372143.11609188572</v>
+        <v>358697.39052595082</v>
       </c>
       <c r="H24" s="15">
-        <v>3528177.7925552498</v>
+        <v>3362100.8638159903</v>
       </c>
       <c r="I24" s="15">
-        <v>92626.486311461151</v>
+        <v>86724.681995816907</v>
       </c>
       <c r="J24" s="15">
-        <v>1062440.9812231972</v>
+        <v>760521.3383055653</v>
       </c>
       <c r="K24" s="15">
-        <v>285441.84035155841</v>
+        <v>254014.41538256884</v>
       </c>
       <c r="L24" s="15">
-        <v>3547913.2735681972</v>
+        <v>3389556.6650699903</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -5581,19 +5575,19 @@
       </c>
       <c r="E31" s="40">
         <f>E12/SUM(E$12:E$24)</f>
-        <v>0.12697530007213642</v>
+        <v>0.12697529992417808</v>
       </c>
       <c r="F31" s="41">
         <f t="shared" ref="F31:L31" si="0">F12/SUM(F$12:F$24)</f>
-        <v>2.5507081050037166E-2</v>
+        <v>2.5507081046277618E-2</v>
       </c>
       <c r="G31" s="41">
         <f t="shared" si="0"/>
-        <v>1.9546803539672712E-3</v>
+        <v>1.9546803539560831E-3</v>
       </c>
       <c r="H31" s="41">
         <f t="shared" si="0"/>
-        <v>2.6767200528738455E-3</v>
+        <v>2.6767200525146502E-3</v>
       </c>
       <c r="I31" s="42">
         <f t="shared" si="0"/>
@@ -5601,7 +5595,7 @@
       </c>
       <c r="J31" s="42">
         <f t="shared" si="0"/>
-        <v>2.209903429909382E-3</v>
+        <v>2.2099034299093816E-3</v>
       </c>
       <c r="K31" s="42">
         <f t="shared" si="0"/>
@@ -5609,7 +5603,7 @@
       </c>
       <c r="L31" s="42">
         <f t="shared" si="0"/>
-        <v>3.7262261828002344E-5</v>
+        <v>3.7262261828002337E-5</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -5624,19 +5618,19 @@
       </c>
       <c r="E32" s="43">
         <f t="shared" ref="E32:L38" si="1">E13/SUM(E$12:E$24)</f>
-        <v>0.20684532361910102</v>
+        <v>0.20684532337807388</v>
       </c>
       <c r="F32" s="44">
         <f t="shared" si="1"/>
-        <v>0.35792082295282462</v>
+        <v>0.35792082290006988</v>
       </c>
       <c r="G32" s="44">
         <f t="shared" si="1"/>
-        <v>0.21119200858645931</v>
+        <v>0.21119200858525053</v>
       </c>
       <c r="H32" s="44">
         <f t="shared" si="1"/>
-        <v>7.4502145100204656E-2</v>
+        <v>7.4502145090207042E-2</v>
       </c>
       <c r="I32" s="38">
         <f t="shared" si="1"/>
@@ -5644,7 +5638,7 @@
       </c>
       <c r="J32" s="38">
         <f t="shared" si="1"/>
-        <v>3.6022970391391129E-2</v>
+        <v>3.6022970391391122E-2</v>
       </c>
       <c r="K32" s="38">
         <f t="shared" si="1"/>
@@ -5652,7 +5646,7 @@
       </c>
       <c r="L32" s="38">
         <f t="shared" si="1"/>
-        <v>2.2444096636223395E-3</v>
+        <v>2.2444096636223391E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -5667,19 +5661,19 @@
       </c>
       <c r="E33" s="43">
         <f t="shared" si="1"/>
-        <v>6.3627341411950479E-3</v>
+        <v>6.3627341337808528E-3</v>
       </c>
       <c r="F33" s="44">
         <f t="shared" si="1"/>
-        <v>6.3699984345161323E-3</v>
+        <v>6.3699984335772435E-3</v>
       </c>
       <c r="G33" s="44">
         <f t="shared" si="1"/>
-        <v>0.18761500503281933</v>
+        <v>0.1876150050317455</v>
       </c>
       <c r="H33" s="44">
         <f t="shared" si="1"/>
-        <v>1.4750073713144565E-2</v>
+        <v>1.4750073711165219E-2</v>
       </c>
       <c r="I33" s="38">
         <f t="shared" si="1"/>
@@ -5687,7 +5681,7 @@
       </c>
       <c r="J33" s="38">
         <f t="shared" si="1"/>
-        <v>1.9543955077004807E-5</v>
+        <v>1.9543955077004804E-5</v>
       </c>
       <c r="K33" s="38">
         <f t="shared" si="1"/>
@@ -5710,19 +5704,19 @@
       </c>
       <c r="E34" s="43">
         <f t="shared" si="1"/>
-        <v>0.16174573238256459</v>
+        <v>0.16174573219408986</v>
       </c>
       <c r="F34" s="44">
         <f t="shared" si="1"/>
-        <v>0.20653248355909165</v>
+        <v>0.20653248352865036</v>
       </c>
       <c r="G34" s="44">
         <f t="shared" si="1"/>
-        <v>0.17577455232090955</v>
+        <v>0.17577455231990347</v>
       </c>
       <c r="H34" s="44">
         <f t="shared" si="1"/>
-        <v>0.29513909719867831</v>
+        <v>0.29513909715907294</v>
       </c>
       <c r="I34" s="38">
         <f t="shared" si="1"/>
@@ -5730,7 +5724,7 @@
       </c>
       <c r="J34" s="38">
         <f t="shared" si="1"/>
-        <v>2.2389044943395234E-2</v>
+        <v>2.238904494339523E-2</v>
       </c>
       <c r="K34" s="38">
         <f t="shared" si="1"/>
@@ -5738,7 +5732,7 @@
       </c>
       <c r="L34" s="38">
         <f t="shared" si="1"/>
-        <v>9.2702861842067011E-3</v>
+        <v>9.2702861842066994E-3</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -5753,19 +5747,19 @@
       </c>
       <c r="E35" s="37">
         <f t="shared" si="1"/>
-        <v>3.4627552815396593E-3</v>
+        <v>3.462755277504673E-3</v>
       </c>
       <c r="F35" s="38">
         <f t="shared" si="1"/>
-        <v>1.2542326391256381E-3</v>
+        <v>1.2542326389407739E-3</v>
       </c>
       <c r="G35" s="38">
         <f t="shared" si="1"/>
-        <v>6.711702573178583E-5</v>
+        <v>6.7117025731401684E-5</v>
       </c>
       <c r="H35" s="38">
         <f t="shared" si="1"/>
-        <v>1.075650310950719E-4</v>
+        <v>1.0756503108063751E-4</v>
       </c>
       <c r="I35" s="44">
         <f t="shared" si="1"/>
@@ -5773,7 +5767,7 @@
       </c>
       <c r="J35" s="44">
         <f t="shared" si="1"/>
-        <v>2.8544313860695385E-2</v>
+        <v>2.8544313860695378E-2</v>
       </c>
       <c r="K35" s="44">
         <f t="shared" si="1"/>
@@ -5781,7 +5775,7 @@
       </c>
       <c r="L35" s="44">
         <f t="shared" si="1"/>
-        <v>7.5169051902419857E-4</v>
+        <v>7.5169051902419846E-4</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -5796,19 +5790,19 @@
       </c>
       <c r="E36" s="37">
         <f t="shared" si="1"/>
-        <v>9.3011606967724324E-3</v>
+        <v>9.3011606859342254E-3</v>
       </c>
       <c r="F36" s="38">
         <f t="shared" si="1"/>
-        <v>4.2153747674315553E-2</v>
+        <v>4.2153747668102419E-2</v>
       </c>
       <c r="G36" s="38">
         <f t="shared" si="1"/>
-        <v>9.375878653446218E-3</v>
+        <v>9.3758786533925543E-3</v>
       </c>
       <c r="H36" s="38">
         <f t="shared" si="1"/>
-        <v>5.448345834571669E-3</v>
+        <v>5.4483458338405429E-3</v>
       </c>
       <c r="I36" s="44">
         <f t="shared" si="1"/>
@@ -5816,7 +5810,7 @@
       </c>
       <c r="J36" s="44">
         <f t="shared" si="1"/>
-        <v>0.2912182233818747</v>
+        <v>0.29121822338187464</v>
       </c>
       <c r="K36" s="44">
         <f t="shared" si="1"/>
@@ -5824,7 +5818,7 @@
       </c>
       <c r="L36" s="44">
         <f t="shared" si="1"/>
-        <v>6.1391440470442128E-2</v>
+        <v>6.1391440470442114E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -5859,7 +5853,7 @@
       </c>
       <c r="J37" s="44">
         <f t="shared" si="1"/>
-        <v>5.6368928974990153E-3</v>
+        <v>5.6368928974990136E-3</v>
       </c>
       <c r="K37" s="44">
         <f t="shared" si="1"/>
@@ -5867,7 +5861,7 @@
       </c>
       <c r="L37" s="44">
         <f t="shared" si="1"/>
-        <v>8.4819950718961618E-3</v>
+        <v>8.48199507189616E-3</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -5882,19 +5876,19 @@
       </c>
       <c r="E38" s="37">
         <f t="shared" si="1"/>
-        <v>7.3433833180007249E-3</v>
+        <v>7.3433833094438249E-3</v>
       </c>
       <c r="F38" s="38">
         <f t="shared" si="1"/>
-        <v>2.4756897623452602E-2</v>
+        <v>2.4756897619803625E-2</v>
       </c>
       <c r="G38" s="38">
         <f t="shared" si="1"/>
-        <v>6.5211864422460904E-3</v>
+        <v>6.5211864422087653E-3</v>
       </c>
       <c r="H38" s="38">
         <f t="shared" si="1"/>
-        <v>4.6160574290974839E-3</v>
+        <v>4.6160574284780454E-3</v>
       </c>
       <c r="I38" s="44">
         <f t="shared" si="1"/>
@@ -5902,7 +5896,7 @@
       </c>
       <c r="J38" s="44">
         <f t="shared" si="1"/>
-        <v>0.18715466642953282</v>
+        <v>0.1871546664295328</v>
       </c>
       <c r="K38" s="44">
         <f t="shared" si="1"/>
@@ -6021,28 +6015,28 @@
       </c>
       <c r="E46" s="40">
         <f t="array" ref="E46:L53">MINVERSE(Additional_calculatations!D144:K151-ModelB_industry_technology!E31:L38)</f>
-        <v>1.1594465487130254</v>
+        <v>1.1594465484938938</v>
       </c>
       <c r="F46" s="41">
-        <v>5.0042988116341135E-2</v>
+        <v>5.0042988094212204E-2</v>
       </c>
       <c r="G46" s="41">
-        <v>1.8085743534373786E-2</v>
+        <v>1.8085743526795768E-2</v>
       </c>
       <c r="H46" s="41">
-        <v>1.0135951714228908E-2</v>
+        <v>1.0135951708949825E-2</v>
       </c>
       <c r="I46" s="42">
-        <v>1.2833098428220112E-2</v>
+        <v>1.2833098425407795E-2</v>
       </c>
       <c r="J46" s="42">
-        <v>7.2897103447442397E-3</v>
+        <v>7.2897103425546934E-3</v>
       </c>
       <c r="K46" s="42">
-        <v>2.7866721839147454E-3</v>
+        <v>2.7866721829331803E-3</v>
       </c>
       <c r="L46" s="42">
-        <v>1.0287959227991575E-3</v>
+        <v>1.0287959224446585E-3</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -6056,28 +6050,28 @@
         <v>8</v>
       </c>
       <c r="E47" s="43">
-        <v>0.42938706481624028</v>
+        <v>0.42938706418518335</v>
       </c>
       <c r="F47" s="44">
-        <v>1.6462740471573292</v>
+        <v>1.6462740469627997</v>
       </c>
       <c r="G47" s="44">
-        <v>0.47059688754412143</v>
+        <v>0.47059688747553469</v>
       </c>
       <c r="H47" s="44">
-        <v>0.18635895101852426</v>
+        <v>0.18635895095851512</v>
       </c>
       <c r="I47" s="38">
-        <v>4.9598468352693804E-2</v>
+        <v>4.9598468340404184E-2</v>
       </c>
       <c r="J47" s="38">
-        <v>9.7759087883870777E-2</v>
+        <v>9.7759087868811892E-2</v>
       </c>
       <c r="K47" s="38">
-        <v>5.2515566663588802E-2</v>
+        <v>5.2515566655785065E-2</v>
       </c>
       <c r="L47" s="38">
-        <v>1.6798403801117225E-2</v>
+        <v>1.6798403798276476E-2</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -6091,28 +6085,28 @@
         <v>9</v>
       </c>
       <c r="E48" s="43">
-        <v>1.9697531378240707E-2</v>
+        <v>1.9697531348653933E-2</v>
       </c>
       <c r="F48" s="44">
-        <v>2.2464426455463926E-2</v>
+        <v>2.2464426446905203E-2</v>
       </c>
       <c r="G48" s="44">
-        <v>1.2430273516316468</v>
+        <v>1.2430273516262074</v>
       </c>
       <c r="H48" s="44">
-        <v>2.8484437221039948E-2</v>
+        <v>2.8484437214478606E-2</v>
       </c>
       <c r="I48" s="38">
-        <v>1.7597483879219259E-3</v>
+        <v>1.7597483872865524E-3</v>
       </c>
       <c r="J48" s="38">
-        <v>2.4017589431615332E-3</v>
+        <v>2.4017589423472913E-3</v>
       </c>
       <c r="K48" s="38">
-        <v>1.5309098235626263E-3</v>
+        <v>1.5309098231082246E-3</v>
       </c>
       <c r="L48" s="38">
-        <v>6.8747716056471401E-4</v>
+        <v>6.8747716037386353E-4</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -6126,28 +6120,28 @@
         <v>10</v>
       </c>
       <c r="E49" s="43">
-        <v>0.39905054912741861</v>
+        <v>0.39905054853039751</v>
       </c>
       <c r="F49" s="44">
-        <v>0.50437320572869226</v>
+        <v>0.50437320555022758</v>
       </c>
       <c r="G49" s="44">
-        <v>0.45435048414569873</v>
+        <v>0.45435048406956852</v>
       </c>
       <c r="H49" s="44">
-        <v>1.4838973741354882</v>
+        <v>1.4838973740204897</v>
       </c>
       <c r="I49" s="38">
-        <v>4.5560154208174657E-2</v>
+        <v>4.5560154195557132E-2</v>
       </c>
       <c r="J49" s="38">
-        <v>8.3689654580062625E-2</v>
+        <v>8.3689654563964835E-2</v>
       </c>
       <c r="K49" s="38">
-        <v>5.6097950376127338E-2</v>
+        <v>5.6097950367280804E-2</v>
       </c>
       <c r="L49" s="38">
-        <v>2.8950341672609174E-2</v>
+        <v>2.8950341669000287E-2</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -6161,28 +6155,28 @@
         <v>7</v>
       </c>
       <c r="E50" s="37">
-        <v>7.4327374747395593E-3</v>
+        <v>7.432737464186049E-3</v>
       </c>
       <c r="F50" s="38">
-        <v>6.8560059035409687E-3</v>
+        <v>6.8560059013458869E-3</v>
       </c>
       <c r="G50" s="38">
-        <v>2.863600749642493E-3</v>
+        <v>2.863600748901924E-3</v>
       </c>
       <c r="H50" s="38">
-        <v>1.4434422311699537E-3</v>
+        <v>1.4434422306059506E-3</v>
       </c>
       <c r="I50" s="44">
-        <v>1.2392121432347711</v>
+        <v>1.2392121432346015</v>
       </c>
       <c r="J50" s="44">
-        <v>5.2022328097164651E-2</v>
+        <v>5.2022328096986467E-2</v>
       </c>
       <c r="K50" s="44">
-        <v>1.3869923841125077E-2</v>
+        <v>1.3869923841036975E-2</v>
       </c>
       <c r="L50" s="44">
-        <v>6.0167450459985691E-3</v>
+        <v>6.0167450459670622E-3</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -6196,28 +6190,28 @@
         <v>8</v>
       </c>
       <c r="E51" s="37">
-        <v>5.022871467361073E-2</v>
+        <v>5.0228714597213335E-2</v>
       </c>
       <c r="F51" s="38">
-        <v>0.11315507238437714</v>
+        <v>0.11315507235225469</v>
       </c>
       <c r="G51" s="38">
-        <v>5.3136400701049823E-2</v>
+        <v>5.3136400690206309E-2</v>
       </c>
       <c r="H51" s="38">
-        <v>2.5557296228504143E-2</v>
+        <v>2.5557296219704945E-2</v>
       </c>
       <c r="I51" s="44">
-        <v>0.38140697666402834</v>
+        <v>0.38140697666229328</v>
       </c>
       <c r="J51" s="44">
-        <v>1.4707529775699439</v>
+        <v>1.4707529775675989</v>
       </c>
       <c r="K51" s="44">
-        <v>0.3543262513393769</v>
+        <v>0.35432625133814494</v>
       </c>
       <c r="L51" s="44">
-        <v>0.13250102132684571</v>
+        <v>0.13250102132640576</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -6231,28 +6225,28 @@
         <v>9</v>
       </c>
       <c r="E52" s="37">
-        <v>7.0343843522661009E-4</v>
+        <v>7.0343843416448607E-4</v>
       </c>
       <c r="F52" s="38">
-        <v>1.4658627407280445E-3</v>
+        <v>1.4658627403073658E-3</v>
       </c>
       <c r="G52" s="38">
-        <v>7.0392550821947984E-4</v>
+        <v>7.0392550807645991E-4</v>
       </c>
       <c r="H52" s="38">
-        <v>3.5281490102933541E-4</v>
+        <v>3.528149009103929E-4</v>
       </c>
       <c r="I52" s="44">
-        <v>1.1962235302848118E-2</v>
+        <v>1.1962235302824718E-2</v>
       </c>
       <c r="J52" s="44">
-        <v>1.2027319540080789E-2</v>
+        <v>1.2027319540049713E-2</v>
       </c>
       <c r="K52" s="44">
-        <v>1.0062974651499117</v>
+        <v>1.0062974651498953</v>
       </c>
       <c r="L52" s="44">
-        <v>1.3083445462351522E-2</v>
+        <v>1.308344546234567E-2</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -6266,28 +6260,28 @@
         <v>10</v>
       </c>
       <c r="E53" s="37">
-        <v>4.4772941788739473E-2</v>
+        <v>4.4772941721081871E-2</v>
       </c>
       <c r="F53" s="38">
-        <v>9.3142057403250877E-2</v>
+        <v>9.3142057376431733E-2</v>
       </c>
       <c r="G53" s="38">
-        <v>4.5799056693534991E-2</v>
+        <v>4.5799056684362204E-2</v>
       </c>
       <c r="H53" s="38">
-        <v>2.366434700871917E-2</v>
+        <v>2.3664347000912248E-2</v>
       </c>
       <c r="I53" s="44">
-        <v>0.36899384949711339</v>
+        <v>0.36899384949561781</v>
       </c>
       <c r="J53" s="44">
-        <v>0.40649964352810414</v>
+        <v>0.40649964352611506</v>
       </c>
       <c r="K53" s="44">
-        <v>0.41187604381712134</v>
+        <v>0.41187604381607634</v>
       </c>
       <c r="L53" s="44">
-        <v>1.4494976408230471</v>
+        <v>1.4494976408226703</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -6388,35 +6382,35 @@
       <c r="D60" s="65"/>
       <c r="E60" s="45">
         <f>SUM(E46:E53)</f>
-        <v>2.1107195264072414</v>
+        <v>2.1107195247747748</v>
       </c>
       <c r="F60" s="46">
         <f t="shared" ref="F60:L60" si="2">SUM(F46:F53)</f>
-        <v>2.4377736658897238</v>
+        <v>2.4377736654244844</v>
       </c>
       <c r="G60" s="46">
         <f t="shared" si="2"/>
-        <v>2.2885634505082879</v>
+        <v>2.288563450329653</v>
       </c>
       <c r="H60" s="46">
         <f t="shared" si="2"/>
-        <v>1.759894614458704</v>
+        <v>1.7598946142545671</v>
       </c>
       <c r="I60" s="46">
         <f t="shared" si="2"/>
-        <v>2.1113266740757717</v>
+        <v>2.1113266740439931</v>
       </c>
       <c r="J60" s="46">
         <f t="shared" si="2"/>
-        <v>2.1324424804871329</v>
+        <v>2.1324424804484292</v>
       </c>
       <c r="K60" s="46">
         <f t="shared" si="2"/>
-        <v>1.8993007831947286</v>
+        <v>1.8993007831742608</v>
       </c>
       <c r="L60" s="46">
         <f t="shared" si="2"/>
-        <v>1.6485638712153332</v>
+        <v>1.6485638712074842</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -6426,35 +6420,35 @@
       <c r="D61" s="67"/>
       <c r="E61" s="47">
         <f>SUMIF($B$46:$B$53,E$57,E46:E53)</f>
-        <v>2.0075816940349251</v>
+        <v>2.0075816925581287</v>
       </c>
       <c r="F61" s="48">
         <f t="shared" ref="F61:L61" si="3">SUMIF($B$46:$B$53,F$57,F46:F53)</f>
-        <v>2.2231546674578264</v>
+        <v>2.2231546670541444</v>
       </c>
       <c r="G61" s="48">
         <f t="shared" si="3"/>
-        <v>2.186060466855841</v>
+        <v>2.1860604666981063</v>
       </c>
       <c r="H61" s="48">
         <f t="shared" si="3"/>
-        <v>1.7088767140892813</v>
+        <v>1.7088767139024332</v>
       </c>
       <c r="I61" s="48">
         <f t="shared" si="3"/>
-        <v>2.0015752046987609</v>
+        <v>2.0015752046953375</v>
       </c>
       <c r="J61" s="48">
         <f t="shared" si="3"/>
-        <v>1.9413022687352934</v>
+        <v>1.9413022687307502</v>
       </c>
       <c r="K61" s="48">
         <f t="shared" si="3"/>
-        <v>1.7863696841475352</v>
+        <v>1.7863696841451535</v>
       </c>
       <c r="L61" s="48">
         <f t="shared" si="3"/>
-        <v>1.6010988526582428</v>
+        <v>1.6010988526573888</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -6464,35 +6458,35 @@
       <c r="D62" s="67"/>
       <c r="E62" s="47">
         <f>SUM(E46:E53)-E61</f>
-        <v>0.10313783237231622</v>
+        <v>0.10313783221664607</v>
       </c>
       <c r="F62" s="48">
         <f t="shared" ref="F62:L62" si="4">SUM(F46:F53)-F61</f>
-        <v>0.21461899843189736</v>
+        <v>0.21461899837033993</v>
       </c>
       <c r="G62" s="48">
         <f t="shared" si="4"/>
-        <v>0.10250298365244692</v>
+        <v>0.10250298363154675</v>
       </c>
       <c r="H62" s="48">
         <f t="shared" si="4"/>
-        <v>5.1017900369422664E-2</v>
+        <v>5.1017900352133827E-2</v>
       </c>
       <c r="I62" s="48">
         <f t="shared" si="4"/>
-        <v>0.10975146937701075</v>
+        <v>0.10975146934865565</v>
       </c>
       <c r="J62" s="48">
         <f t="shared" si="4"/>
-        <v>0.19114021175183948</v>
+        <v>0.19114021171767903</v>
       </c>
       <c r="K62" s="48">
         <f t="shared" si="4"/>
-        <v>0.11293109904719345</v>
+        <v>0.11293109902910725</v>
       </c>
       <c r="L62" s="48">
         <f t="shared" si="4"/>
-        <v>4.7465018557090399E-2</v>
+        <v>4.7465018550095328E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6521,7 +6515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W151"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6773,6 +6769,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="22">
+        <f>SUM(Supply!E8:L8)</f>
         <v>419339.91477028385</v>
       </c>
       <c r="E24" s="23">
@@ -6845,6 +6842,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="25">
+        <f>SUM(Supply!E9:L9)</f>
         <v>7318095.5947802309</v>
       </c>
       <c r="F25" s="25">
@@ -6916,6 +6914,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="25">
+        <f>SUM(Supply!E10:L10)</f>
         <v>1835296.1158707973</v>
       </c>
       <c r="G26" s="25">
@@ -6987,6 +6986,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="25">
+        <f>SUM(Supply!E11:L11)</f>
         <v>13895721.836202566</v>
       </c>
       <c r="H27" s="25">
@@ -7058,6 +7058,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="25">
+        <f>SUM(Supply!E12:L12)</f>
         <v>254829.60387449837</v>
       </c>
       <c r="I28" s="25">
@@ -7129,6 +7130,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="25">
+        <f>SUM(Supply!E13:L13)</f>
         <v>4531056.8481576061</v>
       </c>
       <c r="J29" s="25">
@@ -7200,6 +7202,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="25">
+        <f>SUM(Supply!E14:L14)</f>
         <v>1017210.5071141919</v>
       </c>
       <c r="K30" s="25">
@@ -7271,6 +7274,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="25">
+        <f>SUM(Supply!E15:L15)</f>
         <v>13018694.857161621</v>
       </c>
       <c r="M31" s="4" t="s">
@@ -7371,25 +7375,25 @@
       </c>
       <c r="C36" s="56"/>
       <c r="D36" s="5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>20</v>
@@ -7399,25 +7403,25 @@
       </c>
       <c r="O36" s="56"/>
       <c r="P36" s="5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q36" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="V36" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="W36" s="4" t="s">
         <v>20</v>
@@ -7429,56 +7433,56 @@
       </c>
       <c r="C37" s="58"/>
       <c r="D37" s="11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="N37" s="57" t="s">
         <v>37</v>
       </c>
       <c r="O37" s="58"/>
       <c r="P37" s="11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="Q37" s="12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="R37" s="12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="S37" s="12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="U37" s="12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="V37" s="12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="W37" s="12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -7486,12 +7490,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D38" s="22">
+        <f>SUM(Supply!E8:E15)</f>
         <v>442084.63339509023</v>
       </c>
       <c r="E38" s="23">
@@ -7519,10 +7524,10 @@
         <v>0</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="P38" s="26">
         <f t="array" ref="P38:W45">MINVERSE(D38:K45)</f>
@@ -7555,15 +7560,16 @@
         <v>0</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D39" s="24">
         <v>0</v>
       </c>
       <c r="E39" s="25">
+        <f>SUM(Supply!F8:F15)</f>
         <v>7557272.223811239</v>
       </c>
       <c r="F39" s="25">
@@ -7588,10 +7594,10 @@
         <v>0</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="P39" s="28">
         <v>0</v>
@@ -7623,10 +7629,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D40" s="24">
         <v>0</v>
@@ -7635,6 +7641,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="25">
+        <f>SUM(Supply!G8:G15)</f>
         <v>1819587.5860552089</v>
       </c>
       <c r="G40" s="25">
@@ -7656,10 +7663,10 @@
         <v>0</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="P40" s="28">
         <v>0</v>
@@ -7694,7 +7701,7 @@
         <v>20</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D41" s="24">
         <v>0</v>
@@ -7706,6 +7713,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="25">
+        <f>SUM(Supply!H8:H15)</f>
         <v>13649509.01836234</v>
       </c>
       <c r="H41" s="25">
@@ -7727,7 +7735,7 @@
         <v>20</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="P41" s="28">
         <v>0</v>
@@ -7759,10 +7767,10 @@
         <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D42" s="24">
         <v>0</v>
@@ -7777,6 +7785,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="25">
+        <f>SUM(Supply!I8:I15)</f>
         <v>254150.30272163445</v>
       </c>
       <c r="I42" s="25">
@@ -7792,10 +7801,10 @@
         <v>3</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="P42" s="28">
         <v>0</v>
@@ -7827,10 +7836,10 @@
         <v>3</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D43" s="24">
         <v>0</v>
@@ -7848,6 +7857,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="25">
+        <f>SUM(Supply!J8:J15)</f>
         <v>4547744.7835972272</v>
       </c>
       <c r="J43" s="25">
@@ -7860,10 +7870,10 @@
         <v>3</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="P43" s="28">
         <v>0</v>
@@ -7895,10 +7905,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D44" s="24">
         <v>0</v>
@@ -7919,6 +7929,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="25">
+        <f>SUM(Supply!K8:K15)</f>
         <v>1017210.5071141919</v>
       </c>
       <c r="K44" s="25">
@@ -7928,10 +7939,10 @@
         <v>3</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="P44" s="28">
         <v>0</v>
@@ -7966,7 +7977,7 @@
         <v>20</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D45" s="24">
         <v>0</v>
@@ -7990,6 +8001,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="25">
+        <f>SUM(Supply!L8:L15)</f>
         <v>13002686.222874865</v>
       </c>
       <c r="M45" s="4" t="s">
@@ -7999,7 +8011,7 @@
         <v>20</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="P45" s="28">
         <v>0</v>
@@ -10397,35 +10409,35 @@
       </c>
       <c r="D122" s="14">
         <f>Use!E16</f>
-        <v>0</v>
+        <v>3392.9713519421675</v>
       </c>
       <c r="E122" s="15">
         <f>Use!F16</f>
-        <v>0</v>
+        <v>197334.18558686029</v>
       </c>
       <c r="F122" s="15">
         <f>Use!G16</f>
-        <v>0</v>
+        <v>12743.89411571547</v>
       </c>
       <c r="G122" s="15">
         <f>Use!H16</f>
-        <v>0</v>
+        <v>158355.58075858228</v>
       </c>
       <c r="H122" s="15">
         <f>Use!I16</f>
-        <v>0</v>
+        <v>5907.1633783290745</v>
       </c>
       <c r="I122" s="15">
         <f>Use!J16</f>
-        <v>0</v>
+        <v>308796.03558555245</v>
       </c>
       <c r="J122" s="15">
         <f>Use!K16</f>
-        <v>0</v>
+        <v>31427.424968989566</v>
       </c>
       <c r="K122" s="15">
         <f>Use!L16</f>
-        <v>0</v>
+        <v>151474.85676760226</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -10437,19 +10449,19 @@
       </c>
       <c r="D123" s="14">
         <f>Use!E17</f>
-        <v>0</v>
+        <v>6710.2411205275657</v>
       </c>
       <c r="E123" s="15">
         <f>Use!F17</f>
-        <v>0</v>
+        <v>74985.055966575514</v>
       </c>
       <c r="F123" s="15">
         <f>Use!G17</f>
-        <v>0</v>
+        <v>17099.420776746472</v>
       </c>
       <c r="G123" s="15">
         <f>Use!H17</f>
-        <v>0</v>
+        <v>271017.71884496155</v>
       </c>
       <c r="H123" s="15">
         <f>Use!I17</f>
@@ -10477,35 +10489,35 @@
       </c>
       <c r="D124" s="14">
         <f>Use!E18</f>
-        <v>43763.978517646319</v>
+        <v>58933.521905901594</v>
       </c>
       <c r="E124" s="15">
         <f>Use!F18</f>
-        <v>1261728.1978450278</v>
+        <v>1243388.8572053353</v>
       </c>
       <c r="F124" s="15">
         <f>Use!G18</f>
-        <v>367397.85566209425</v>
+        <v>378882.97400441696</v>
       </c>
       <c r="G124" s="15">
         <f>Use!H18</f>
-        <v>4833323.2046840414</v>
+        <v>4286444.7468843479</v>
       </c>
       <c r="H124" s="15">
         <f>Use!I18</f>
-        <v>19560.027310772057</v>
+        <v>31109.987250275444</v>
       </c>
       <c r="I124" s="15">
         <f>Use!J18</f>
-        <v>857396.56827209215</v>
+        <v>898321.88750478718</v>
       </c>
       <c r="J124" s="15">
         <f>Use!K18</f>
-        <v>250974.27487646061</v>
+        <v>271453.90956404991</v>
       </c>
       <c r="K124" s="15">
         <f>Use!L18</f>
-        <v>4640128.2654448878</v>
+        <v>4359561.9561253022</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
@@ -10517,35 +10529,35 @@
       </c>
       <c r="D125" s="14">
         <f>Use!E19</f>
-        <v>0</v>
+        <v>-21879.784508782846</v>
       </c>
       <c r="E125" s="15">
         <f>Use!F19</f>
-        <v>0</v>
+        <v>-56645.715326882782</v>
       </c>
       <c r="F125" s="15">
         <f>Use!G19</f>
-        <v>0</v>
+        <v>-28584.539119069173</v>
       </c>
       <c r="G125" s="15">
         <f>Use!H19</f>
-        <v>0</v>
+        <v>275860.7389547326</v>
       </c>
       <c r="H125" s="15">
         <f>Use!I19</f>
-        <v>0</v>
+        <v>-11549.959939503386</v>
       </c>
       <c r="I125" s="15">
         <f>Use!J19</f>
-        <v>0</v>
+        <v>-40925.319232695016</v>
       </c>
       <c r="J125" s="15">
         <f>Use!K19</f>
-        <v>0</v>
+        <v>-20479.634687589296</v>
       </c>
       <c r="K125" s="15">
         <f>Use!L19</f>
-        <v>0</v>
+        <v>280566.30931958527</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -10557,35 +10569,35 @@
       </c>
       <c r="D126" s="14">
         <f>Use!E20</f>
-        <v>167517.38477739022</v>
+        <v>164124.41394568497</v>
       </c>
       <c r="E126" s="15">
         <f>Use!F20</f>
-        <v>1240315.4284159234</v>
+        <v>1042981.2439283638</v>
       </c>
       <c r="F126" s="15">
         <f>Use!G20</f>
-        <v>367285.61832482147</v>
+        <v>354541.724209106</v>
       </c>
       <c r="G126" s="15">
         <f>Use!H20</f>
-        <v>3498020.896852497</v>
+        <v>3339665.3179168464</v>
       </c>
       <c r="H126" s="15">
         <f>Use!I20</f>
-        <v>92545.603780070684</v>
+        <v>86638.440401741609</v>
       </c>
       <c r="I126" s="15">
         <f>Use!J20</f>
-        <v>1062327.7036943426</v>
+        <v>753531.66810879018</v>
       </c>
       <c r="J126" s="15">
         <f>Use!K20</f>
-        <v>285441.84035155841</v>
+        <v>254014.41538256884</v>
       </c>
       <c r="K126" s="15">
         <f>Use!L20</f>
-        <v>3548107.4336284427</v>
+        <v>3396632.5768608404</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -10662,28 +10674,28 @@
       </c>
       <c r="D133" s="37">
         <f t="array" ref="D133:K137">MMULT(D122:K126,P38:W45)</f>
-        <v>0</v>
+        <v>7.6749361901251043E-3</v>
       </c>
       <c r="E133" s="38">
-        <v>0</v>
+        <v>2.6111827090878812E-2</v>
       </c>
       <c r="F133" s="38">
-        <v>0</v>
+        <v>7.0037266759682111E-3</v>
       </c>
       <c r="G133" s="38">
-        <v>0</v>
+        <v>1.1601558748050975E-2</v>
       </c>
       <c r="H133" s="38">
-        <v>0</v>
+        <v>2.3242794972387137E-2</v>
       </c>
       <c r="I133" s="38">
-        <v>0</v>
+        <v>6.7900915790023164E-2</v>
       </c>
       <c r="J133" s="38">
-        <v>0</v>
+        <v>3.0895694400708277E-2</v>
       </c>
       <c r="K133" s="38">
-        <v>0</v>
+        <v>1.1649504892390731E-2</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
@@ -10694,16 +10706,16 @@
         <v>41</v>
       </c>
       <c r="D134" s="37">
-        <v>0</v>
+        <v>1.5178634617979664E-2</v>
       </c>
       <c r="E134" s="38">
-        <v>0</v>
+        <v>9.9222383084619763E-3</v>
       </c>
       <c r="F134" s="38">
-        <v>0</v>
+        <v>9.397415605487458E-3</v>
       </c>
       <c r="G134" s="38">
-        <v>0</v>
+        <v>1.9855492126520321E-2</v>
       </c>
       <c r="H134" s="38">
         <v>0</v>
@@ -10726,28 +10738,28 @@
         <v>42</v>
       </c>
       <c r="D135" s="37">
-        <v>9.8994570748932878E-2</v>
+        <v>0.13330823433809066</v>
       </c>
       <c r="E135" s="38">
-        <v>0.1669555046422187</v>
+        <v>0.1645287903335943</v>
       </c>
       <c r="F135" s="38">
-        <v>0.20191270729572172</v>
+        <v>0.20822464217060291</v>
       </c>
       <c r="G135" s="38">
-        <v>0.35410234889635178</v>
+        <v>0.31403655187288437</v>
       </c>
       <c r="H135" s="38">
-        <v>7.6962439553714596E-2</v>
+        <v>0.12240783078802613</v>
       </c>
       <c r="I135" s="38">
-        <v>0.18853225259353687</v>
+        <v>0.19753128863889813</v>
       </c>
       <c r="J135" s="38">
-        <v>0.24672796153912149</v>
+        <v>0.26686109479360354</v>
       </c>
       <c r="K135" s="38">
-        <v>0.35685920477583949</v>
+        <v>0.33528163960888174</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
@@ -10758,28 +10770,28 @@
         <v>40</v>
       </c>
       <c r="D136" s="37">
-        <v>0</v>
+        <v>-4.9492298207137457E-2</v>
       </c>
       <c r="E136" s="38">
-        <v>0</v>
+        <v>-7.4955239998375422E-3</v>
       </c>
       <c r="F136" s="38">
-        <v>0</v>
+        <v>-1.570935048036862E-2</v>
       </c>
       <c r="G136" s="38">
-        <v>0</v>
+        <v>2.0210304896947143E-2</v>
       </c>
       <c r="H136" s="38">
-        <v>0</v>
+        <v>-4.5445391234311523E-2</v>
       </c>
       <c r="I136" s="38">
-        <v>0</v>
+        <v>-8.9990360453612427E-3</v>
       </c>
       <c r="J136" s="38">
-        <v>0</v>
+        <v>-2.0133133254482058E-2</v>
       </c>
       <c r="K136" s="38">
-        <v>0</v>
+        <v>2.1577565166957687E-2</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
@@ -10790,28 +10802,28 @@
         <v>39</v>
       </c>
       <c r="D137" s="37">
-        <v>0.3789260519889644</v>
+        <v>0.37125111697562052</v>
       </c>
       <c r="E137" s="38">
-        <v>0.16412210539511499</v>
+        <v>0.13801027844969882</v>
       </c>
       <c r="F137" s="38">
-        <v>0.20185102445168995</v>
+        <v>0.19484729777572177</v>
       </c>
       <c r="G137" s="38">
-        <v>0.25627448519552593</v>
+        <v>0.24467292658102788</v>
       </c>
       <c r="H137" s="38">
-        <v>0.3641372950927938</v>
+        <v>0.34089450012040667</v>
       </c>
       <c r="I137" s="38">
-        <v>0.23359439771685042</v>
+        <v>0.16569348192682726</v>
       </c>
       <c r="J137" s="38">
-        <v>0.28061235934472584</v>
+        <v>0.24971666494401756</v>
       </c>
       <c r="K137" s="38">
-        <v>0.27287495620608493</v>
+        <v>0.26122545131369423</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>